<commit_message>
start of relative ab on fish data
</commit_message>
<xml_diff>
--- a/FishLandings/data/fishbase.xlsx
+++ b/FishLandings/data/fishbase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/Kenya_SamakiSalama/FishLandings/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877ECEE3-E6AB-E549-97E3-44E66EBF13BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB124CF2-37C9-BD4F-9868-50A3C89EB000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21080" yWindow="3920" windowWidth="10000" windowHeight="12660" xr2:uid="{607C05E3-912F-FB47-AACE-D6546F681BC3}"/>
+    <workbookView xWindow="6880" yWindow="2580" windowWidth="25200" windowHeight="15660" xr2:uid="{607C05E3-912F-FB47-AACE-D6546F681BC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,22 +35,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>scientific_name</t>
+  </si>
+  <si>
+    <t>Leptoscarus vaigiensis</t>
+  </si>
+  <si>
+    <t>Lethrinus nebulosus</t>
+  </si>
+  <si>
+    <t>Scarus ghobban</t>
+  </si>
+  <si>
+    <t>Siganus canaliculutus</t>
+  </si>
+  <si>
+    <t>Siganus sutor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Monaco"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -73,8 +94,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,15 +411,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27ABF6E-FCDE-A64A-8E31-FB070AB67392}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
@@ -407,6 +429,31 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CUE up to issue with FishBaseR
</commit_message>
<xml_diff>
--- a/FishLandings/data/fishbase.xlsx
+++ b/FishLandings/data/fishbase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/Kenya_SamakiSalama/FishLandings/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3ED682-FA6B-5345-A3BB-DA29FB0069CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33DF57F-328D-3A4B-A5AA-8AE24F86501B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5900" yWindow="460" windowWidth="27680" windowHeight="19540" xr2:uid="{607C05E3-912F-FB47-AACE-D6546F681BC3}"/>
   </bookViews>
@@ -622,11 +622,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
-    <numFmt numFmtId="172" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -647,6 +647,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -675,27 +683,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1010,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27ABF6E-FCDE-A64A-8E31-FB070AB67392}">
   <dimension ref="A1:BD36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AP26" sqref="AP26"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="AZ28" sqref="AZ28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4620,7 +4631,7 @@
       <c r="BC21" t="s">
         <v>177</v>
       </c>
-      <c r="BD21" t="s">
+      <c r="BD21" s="15" t="s">
         <v>178</v>
       </c>
     </row>
@@ -4790,7 +4801,7 @@
       <c r="BC22" t="s">
         <v>177</v>
       </c>
-      <c r="BD22" t="s">
+      <c r="BD22" s="15" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5741,6 +5752,10 @@
       <c r="L36" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="BD21" r:id="rId1" xr:uid="{0855E8CE-BF5D-FE4C-B242-2206D93E6385}"/>
+    <hyperlink ref="BD22" r:id="rId2" xr:uid="{D17C73AE-DE32-7A49-92CA-00525E9614E3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updated figures and maturity info
</commit_message>
<xml_diff>
--- a/FishLandings/data/fishbase.xlsx
+++ b/FishLandings/data/fishbase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/Kenya_SamakiSalama/FishLandings/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BC5030-0E00-3646-AE00-CAA2F172365F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBBE165-5B3F-6449-AF4B-795B08946C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{607C05E3-912F-FB47-AACE-D6546F681BC3}"/>
+    <workbookView xWindow="5740" yWindow="460" windowWidth="38400" windowHeight="19720" xr2:uid="{607C05E3-912F-FB47-AACE-D6546F681BC3}"/>
   </bookViews>
   <sheets>
     <sheet name="life history" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="306">
   <si>
     <t>scientific_name</t>
   </si>
@@ -780,9 +780,6 @@
     <t>https://www.fishbase.se/popdyn/LWRelationshipList.php?ID=7878&amp;GenusName=Parupeneus&amp;SpeciesName=macronemus&amp;fc=332</t>
   </si>
   <si>
-    <t>6.2-27.5</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/popdyn/LLRelationshipList.php?ID=7703&amp;GenusName=Plectorhinchus&amp;SpeciesName=gaterinus&amp;fc=327</t>
   </si>
   <si>
@@ -792,9 +789,6 @@
     <t>https://www.fishbase.se/popdyn/LWRelationshipList.php?ID=7626&amp;GenusName=Plectorhinchus&amp;SpeciesName=sordidus&amp;fc=327</t>
   </si>
   <si>
-    <t>6.1-36.6</t>
-  </si>
-  <si>
     <t>https://www.fishbase.se/popdyn/LLRelationshipList.php?ID=25706&amp;GenusName=Plectorhinchus&amp;SpeciesName=vittatus&amp;fc=327</t>
   </si>
   <si>
@@ -832,6 +826,138 @@
   </si>
   <si>
     <t>https://www.fishbase.se/popdyn/LWRelationshipList.php?ID=1288&amp;GenusName=Trichiurus&amp;SpeciesName=lepturus&amp;fc=415</t>
+  </si>
+  <si>
+    <t>Acanthurus nigrofuscus</t>
+  </si>
+  <si>
+    <t>Cantherhines sandwichiensis</t>
+  </si>
+  <si>
+    <t>Chaetodon auriga</t>
+  </si>
+  <si>
+    <t>Chaetodon selene</t>
+  </si>
+  <si>
+    <t>Lethrinus mahsena</t>
+  </si>
+  <si>
+    <t>Parupeneus indicus</t>
+  </si>
+  <si>
+    <t>Plectorhinchus flavomaculatus</t>
+  </si>
+  <si>
+    <t>Scarus psittacus</t>
+  </si>
+  <si>
+    <t>Scarus russelii</t>
+  </si>
+  <si>
+    <t>Siganus stellatus</t>
+  </si>
+  <si>
+    <t>Brown surgeonfish</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/KeyfactsSummary_1.php?ID=4739&amp;GenusName=Acanthurus&amp;SpeciesName=nigrofuscus&amp;vStockCode=4963&amp;fc=412</t>
+  </si>
+  <si>
+    <t>5.7-16.5</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/LWRelationshipList.php?ID=4739&amp;GenusName=Acanthurus&amp;SpeciesName=nigrofuscus&amp;fc=412</t>
+  </si>
+  <si>
+    <t>Sandwich isle file</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/KeyfactsSummary_2v2.php?ID=7835&amp;GenusName=Cantherhines&amp;SpeciesName=sandwichiensis&amp;vStockCode=8145&amp;fc=517</t>
+  </si>
+  <si>
+    <t>Threadfin butterflyfish</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/KeyfactsSummary_1.php?ID=5557&amp;GenusName=Chaetodon&amp;SpeciesName=auriga&amp;vStockCode=5847&amp;fc=343</t>
+  </si>
+  <si>
+    <t>Yellow-dotted butterflyfish</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/KeyfactsSummary_2v2.php?ID=6634&amp;GenusName=Chaetodon&amp;SpeciesName=selene&amp;vStockCode=6954&amp;fc=343</t>
+  </si>
+  <si>
+    <t>4.5-19</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/LWRelationshipList.php?ID=5557&amp;GenusName=Chaetodon&amp;SpeciesName=auriga&amp;fc=343</t>
+  </si>
+  <si>
+    <t>Sky emperor</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/KeyfactsSummary_1.php?ID=1843&amp;GenusName=Lethrinus&amp;SpeciesName=mahsena&amp;vStockCode=2039&amp;fc=328</t>
+  </si>
+  <si>
+    <t>Indian goatfish</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/KeyfactsSummary_2v2.php?ID=5992&amp;GenusName=Parupeneus&amp;SpeciesName=indicus&amp;vStockCode=6301&amp;fc=332</t>
+  </si>
+  <si>
+    <t>8.5-31.6</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/LWRelationshipList.php?ID=5992&amp;GenusName=Parupeneus&amp;SpeciesName=indicus&amp;fc=332</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/LWRelationshipList.php?ID=1843&amp;GenusName=Lethrinus&amp;SpeciesName=mahsena&amp;fc=328</t>
+  </si>
+  <si>
+    <t>Lemonfish</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/KeyfactsSummary_2v2.php?ID=7625&amp;GenusName=Plectorhinchus&amp;SpeciesName=flavomaculatus&amp;vStockCode=7933&amp;fc=327</t>
+  </si>
+  <si>
+    <t>17.5-49</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/LWRelationshipList.php?ID=7625&amp;GenusName=Plectorhinchus&amp;SpeciesName=flavomaculatus&amp;fc=327</t>
+  </si>
+  <si>
+    <t>Common parrotfish</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/KeyfactsSummary_1.php?ID=5553&amp;GenusName=Scarus&amp;SpeciesName=psittacus&amp;vStockCode=5843&amp;fc=364</t>
+  </si>
+  <si>
+    <t>18.0-34.0</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/LWRelationshipList.php?ID=5553&amp;GenusName=Scarus&amp;SpeciesName=psittacus&amp;fc=364</t>
+  </si>
+  <si>
+    <t>Eclipse parrotfish</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/KeyfactsSummary_2v2.php?ID=7912&amp;GenusName=Scarus&amp;SpeciesName=russelii&amp;vStockCode=8223&amp;fc=364</t>
+  </si>
+  <si>
+    <t>Brown-spotted spinefoot</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/KeyfactsSummary_2v2.php?ID=4622&amp;GenusName=Siganus&amp;SpeciesName=stellatus&amp;vStockCode=4809&amp;fc=413</t>
+  </si>
+  <si>
+    <t>12.0-34.0</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/popdyn/LWRelationshipList.php?ID=4622&amp;GenusName=Siganus&amp;SpeciesName=stellatus&amp;fc=413</t>
   </si>
 </sst>
 </file>
@@ -1240,15 +1366,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27ABF6E-FCDE-A64A-8E31-FB070AB67392}">
-  <dimension ref="A1:BD27"/>
+  <dimension ref="A1:BD37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="2" max="2" width="29.5" customWidth="1"/>
     <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
@@ -5876,6 +6002,1706 @@
         <v>192</v>
       </c>
     </row>
+    <row r="28" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>262</v>
+      </c>
+      <c r="B28" t="s">
+        <v>272</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>25</v>
+      </c>
+      <c r="F28">
+        <v>21</v>
+      </c>
+      <c r="G28">
+        <v>12</v>
+      </c>
+      <c r="H28" t="s">
+        <v>115</v>
+      </c>
+      <c r="I28" t="s">
+        <v>115</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="K28">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="L28">
+        <v>1.77</v>
+      </c>
+      <c r="M28">
+        <v>1.17</v>
+      </c>
+      <c r="N28" s="3">
+        <v>2.67</v>
+      </c>
+      <c r="O28" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="P28" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>115</v>
+      </c>
+      <c r="R28">
+        <v>1.5</v>
+      </c>
+      <c r="S28" t="s">
+        <v>115</v>
+      </c>
+      <c r="T28" t="s">
+        <v>115</v>
+      </c>
+      <c r="U28">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="V28" t="s">
+        <v>115</v>
+      </c>
+      <c r="W28" t="s">
+        <v>115</v>
+      </c>
+      <c r="X28">
+        <v>7.8</v>
+      </c>
+      <c r="Y28">
+        <v>5.8</v>
+      </c>
+      <c r="Z28">
+        <v>10.4</v>
+      </c>
+      <c r="AA28">
+        <v>7.1</v>
+      </c>
+      <c r="AB28">
+        <v>6</v>
+      </c>
+      <c r="AC28">
+        <v>8.4</v>
+      </c>
+      <c r="AD28" s="4">
+        <v>12</v>
+      </c>
+      <c r="AE28">
+        <v>49</v>
+      </c>
+      <c r="AF28">
+        <v>2.64E-2</v>
+      </c>
+      <c r="AG28" s="6">
+        <v>3.0283699999999998</v>
+      </c>
+      <c r="AH28" s="7">
+        <v>49</v>
+      </c>
+      <c r="AI28">
+        <v>1.2</v>
+      </c>
+      <c r="AJ28">
+        <v>7.7</v>
+      </c>
+      <c r="AK28" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL28" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM28" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN28">
+        <v>2.2700000000000001E-2</v>
+      </c>
+      <c r="AO28">
+        <v>4.8</v>
+      </c>
+      <c r="AP28">
+        <v>0.5</v>
+      </c>
+      <c r="AQ28">
+        <v>0.67</v>
+      </c>
+      <c r="AR28">
+        <v>0.59</v>
+      </c>
+      <c r="AS28">
+        <v>3.59</v>
+      </c>
+      <c r="AT28">
+        <v>2.59</v>
+      </c>
+      <c r="AU28">
+        <v>7.18</v>
+      </c>
+      <c r="AV28">
+        <v>4.8</v>
+      </c>
+      <c r="AW28">
+        <v>2</v>
+      </c>
+      <c r="AX28" t="s">
+        <v>115</v>
+      </c>
+      <c r="AY28">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="AZ28">
+        <v>49</v>
+      </c>
+      <c r="BA28">
+        <v>26</v>
+      </c>
+      <c r="BB28">
+        <v>1.32</v>
+      </c>
+      <c r="BC28" t="s">
+        <v>116</v>
+      </c>
+      <c r="BD28" s="8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="29" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>263</v>
+      </c>
+      <c r="B29" t="s">
+        <v>276</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>73</v>
+      </c>
+      <c r="F29">
+        <v>19.3</v>
+      </c>
+      <c r="G29">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="H29" t="s">
+        <v>115</v>
+      </c>
+      <c r="I29" t="s">
+        <v>115</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="K29" t="s">
+        <v>115</v>
+      </c>
+      <c r="L29">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M29">
+        <v>0.73</v>
+      </c>
+      <c r="N29" s="3">
+        <v>1.67</v>
+      </c>
+      <c r="O29" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="P29">
+        <v>0.5</v>
+      </c>
+      <c r="Q29">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R29">
+        <v>2.1</v>
+      </c>
+      <c r="S29" t="s">
+        <v>115</v>
+      </c>
+      <c r="T29" t="s">
+        <v>115</v>
+      </c>
+      <c r="U29">
+        <v>1.5</v>
+      </c>
+      <c r="V29">
+        <v>1.2</v>
+      </c>
+      <c r="W29">
+        <v>2</v>
+      </c>
+      <c r="X29">
+        <v>12.5</v>
+      </c>
+      <c r="Y29">
+        <v>9.4</v>
+      </c>
+      <c r="Z29">
+        <v>16.8</v>
+      </c>
+      <c r="AA29">
+        <v>12.3</v>
+      </c>
+      <c r="AB29">
+        <v>10.4</v>
+      </c>
+      <c r="AC29">
+        <v>14.6</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>115</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>115</v>
+      </c>
+      <c r="AH29" t="s">
+        <v>115</v>
+      </c>
+      <c r="AI29" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ29" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK29" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL29" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM29" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN29">
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="AO29">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="AP29">
+        <v>0.5</v>
+      </c>
+      <c r="AQ29">
+        <v>0.66</v>
+      </c>
+      <c r="AR29">
+        <v>0.59</v>
+      </c>
+      <c r="AS29">
+        <v>2.14</v>
+      </c>
+      <c r="AT29">
+        <v>1.55</v>
+      </c>
+      <c r="AU29">
+        <v>4.28</v>
+      </c>
+      <c r="AV29">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="AW29">
+        <v>2.7</v>
+      </c>
+      <c r="AX29">
+        <v>0.21</v>
+      </c>
+      <c r="AY29">
+        <v>41.8</v>
+      </c>
+      <c r="AZ29">
+        <v>84.9</v>
+      </c>
+      <c r="BA29">
+        <v>25</v>
+      </c>
+      <c r="BB29">
+        <v>1.32</v>
+      </c>
+      <c r="BC29" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD29" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="30" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>264</v>
+      </c>
+      <c r="B30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>60</v>
+      </c>
+      <c r="F30">
+        <v>23</v>
+      </c>
+      <c r="G30">
+        <v>15.4</v>
+      </c>
+      <c r="H30" t="s">
+        <v>115</v>
+      </c>
+      <c r="I30" t="s">
+        <v>115</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="K30">
+        <v>2.16</v>
+      </c>
+      <c r="L30">
+        <v>1.42</v>
+      </c>
+      <c r="M30">
+        <v>0.94</v>
+      </c>
+      <c r="N30" s="3">
+        <v>2.14</v>
+      </c>
+      <c r="O30" s="4">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="P30" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>115</v>
+      </c>
+      <c r="R30">
+        <v>1.8</v>
+      </c>
+      <c r="S30" t="s">
+        <v>115</v>
+      </c>
+      <c r="T30" t="s">
+        <v>115</v>
+      </c>
+      <c r="U30">
+        <v>1.3</v>
+      </c>
+      <c r="V30" t="s">
+        <v>115</v>
+      </c>
+      <c r="W30" t="s">
+        <v>115</v>
+      </c>
+      <c r="X30">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="Y30">
+        <v>7.3</v>
+      </c>
+      <c r="Z30">
+        <v>13</v>
+      </c>
+      <c r="AA30">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AB30">
+        <v>7.8</v>
+      </c>
+      <c r="AC30">
+        <v>10.9</v>
+      </c>
+      <c r="AD30" s="4">
+        <v>15.4</v>
+      </c>
+      <c r="AE30">
+        <v>100.2</v>
+      </c>
+      <c r="AF30">
+        <v>3.1199999999999999E-2</v>
+      </c>
+      <c r="AG30" s="6">
+        <v>2.9529999999999998</v>
+      </c>
+      <c r="AH30" s="7">
+        <v>101</v>
+      </c>
+      <c r="AI30">
+        <v>2.6</v>
+      </c>
+      <c r="AJ30">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="AK30" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL30" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM30" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN30">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="AO30">
+        <v>6.2</v>
+      </c>
+      <c r="AP30">
+        <v>0.5</v>
+      </c>
+      <c r="AQ30">
+        <v>0.68</v>
+      </c>
+      <c r="AR30">
+        <v>0.6</v>
+      </c>
+      <c r="AS30">
+        <v>3.02</v>
+      </c>
+      <c r="AT30">
+        <v>2.13</v>
+      </c>
+      <c r="AU30">
+        <v>6.04</v>
+      </c>
+      <c r="AV30">
+        <v>6.2</v>
+      </c>
+      <c r="AW30">
+        <v>3.7</v>
+      </c>
+      <c r="AX30">
+        <v>0.3</v>
+      </c>
+      <c r="AY30">
+        <v>13.1</v>
+      </c>
+      <c r="AZ30">
+        <v>100.2</v>
+      </c>
+      <c r="BA30">
+        <v>27</v>
+      </c>
+      <c r="BB30">
+        <v>1.32</v>
+      </c>
+      <c r="BC30" t="s">
+        <v>123</v>
+      </c>
+      <c r="BD30" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="31" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>265</v>
+      </c>
+      <c r="B31" t="s">
+        <v>280</v>
+      </c>
+      <c r="C31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>50</v>
+      </c>
+      <c r="F31">
+        <v>16</v>
+      </c>
+      <c r="G31">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="H31" t="s">
+        <v>115</v>
+      </c>
+      <c r="I31" t="s">
+        <v>115</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K31" t="s">
+        <v>115</v>
+      </c>
+      <c r="L31">
+        <v>1.62</v>
+      </c>
+      <c r="M31">
+        <v>1.07</v>
+      </c>
+      <c r="N31" s="3">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="O31" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="P31">
+        <v>0.3</v>
+      </c>
+      <c r="Q31">
+        <v>0.7</v>
+      </c>
+      <c r="R31">
+        <v>1.4</v>
+      </c>
+      <c r="S31" t="s">
+        <v>115</v>
+      </c>
+      <c r="T31" t="s">
+        <v>115</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="V31">
+        <v>0.8</v>
+      </c>
+      <c r="W31">
+        <v>1.3</v>
+      </c>
+      <c r="X31">
+        <v>10.6</v>
+      </c>
+      <c r="Y31">
+        <v>7.9</v>
+      </c>
+      <c r="Z31">
+        <v>14.2</v>
+      </c>
+      <c r="AA31">
+        <v>10.1</v>
+      </c>
+      <c r="AB31">
+        <v>8.6</v>
+      </c>
+      <c r="AC31">
+        <v>12</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>115</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>115</v>
+      </c>
+      <c r="AH31" t="s">
+        <v>115</v>
+      </c>
+      <c r="AI31" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ31" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK31" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL31" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM31" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN31">
+        <v>2.76E-2</v>
+      </c>
+      <c r="AO31">
+        <v>6.8</v>
+      </c>
+      <c r="AP31">
+        <v>0.5</v>
+      </c>
+      <c r="AQ31">
+        <v>0.65</v>
+      </c>
+      <c r="AR31">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AS31">
+        <v>3.01</v>
+      </c>
+      <c r="AT31">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AU31">
+        <v>6.02</v>
+      </c>
+      <c r="AV31">
+        <v>6.8</v>
+      </c>
+      <c r="AW31">
+        <v>2.7</v>
+      </c>
+      <c r="AX31">
+        <v>0.24</v>
+      </c>
+      <c r="AY31">
+        <v>13.8</v>
+      </c>
+      <c r="AZ31">
+        <v>48.3</v>
+      </c>
+      <c r="BA31">
+        <v>25</v>
+      </c>
+      <c r="BB31">
+        <v>1.32</v>
+      </c>
+      <c r="BC31" t="s">
+        <v>123</v>
+      </c>
+      <c r="BD31" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="32" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>266</v>
+      </c>
+      <c r="B32" t="s">
+        <v>284</v>
+      </c>
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>100</v>
+      </c>
+      <c r="F32">
+        <v>65</v>
+      </c>
+      <c r="G32">
+        <v>64.5</v>
+      </c>
+      <c r="H32" t="s">
+        <v>115</v>
+      </c>
+      <c r="I32" t="s">
+        <v>115</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K32">
+        <v>2.62</v>
+      </c>
+      <c r="L32">
+        <v>0.26</v>
+      </c>
+      <c r="M32">
+        <v>0.17</v>
+      </c>
+      <c r="N32" s="3">
+        <v>0.39</v>
+      </c>
+      <c r="O32" s="4">
+        <v>28.6</v>
+      </c>
+      <c r="P32" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>115</v>
+      </c>
+      <c r="R32">
+        <v>8.6</v>
+      </c>
+      <c r="S32" t="s">
+        <v>115</v>
+      </c>
+      <c r="T32" t="s">
+        <v>115</v>
+      </c>
+      <c r="U32">
+        <v>6.5</v>
+      </c>
+      <c r="V32" t="s">
+        <v>115</v>
+      </c>
+      <c r="W32" t="s">
+        <v>115</v>
+      </c>
+      <c r="X32">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="Y32">
+        <v>26.3</v>
+      </c>
+      <c r="Z32">
+        <v>47.2</v>
+      </c>
+      <c r="AA32">
+        <v>40.9</v>
+      </c>
+      <c r="AB32">
+        <v>34.6</v>
+      </c>
+      <c r="AC32">
+        <v>48.4</v>
+      </c>
+      <c r="AD32" s="4">
+        <v>64.5</v>
+      </c>
+      <c r="AE32">
+        <v>6272</v>
+      </c>
+      <c r="AF32">
+        <v>1.2E-2</v>
+      </c>
+      <c r="AG32" s="6">
+        <v>3.16</v>
+      </c>
+      <c r="AH32" s="7">
+        <v>6272</v>
+      </c>
+      <c r="AI32">
+        <v>182.5</v>
+      </c>
+      <c r="AJ32">
+        <v>1140.8</v>
+      </c>
+      <c r="AK32">
+        <v>66615</v>
+      </c>
+      <c r="AL32">
+        <v>26700</v>
+      </c>
+      <c r="AM32">
+        <v>166200</v>
+      </c>
+      <c r="AN32">
+        <v>1.77E-2</v>
+      </c>
+      <c r="AO32">
+        <v>25.8</v>
+      </c>
+      <c r="AP32">
+        <v>0.5</v>
+      </c>
+      <c r="AQ32">
+        <v>0.71</v>
+      </c>
+      <c r="AR32">
+        <v>0.61</v>
+      </c>
+      <c r="AS32">
+        <v>0.64</v>
+      </c>
+      <c r="AT32">
+        <v>0.41</v>
+      </c>
+      <c r="AU32">
+        <v>1.28</v>
+      </c>
+      <c r="AV32">
+        <v>25.8</v>
+      </c>
+      <c r="AW32">
+        <v>3.4</v>
+      </c>
+      <c r="AX32">
+        <v>0.42</v>
+      </c>
+      <c r="AY32">
+        <v>5.7</v>
+      </c>
+      <c r="AZ32">
+        <v>6271.8</v>
+      </c>
+      <c r="BA32">
+        <v>27</v>
+      </c>
+      <c r="BB32">
+        <v>1.32</v>
+      </c>
+      <c r="BC32" t="s">
+        <v>123</v>
+      </c>
+      <c r="BD32" s="8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="33" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>267</v>
+      </c>
+      <c r="B33" t="s">
+        <v>286</v>
+      </c>
+      <c r="C33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <v>30</v>
+      </c>
+      <c r="F33">
+        <v>45</v>
+      </c>
+      <c r="G33">
+        <v>46.9</v>
+      </c>
+      <c r="H33" t="s">
+        <v>115</v>
+      </c>
+      <c r="I33" t="s">
+        <v>115</v>
+      </c>
+      <c r="J33" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="K33" t="s">
+        <v>115</v>
+      </c>
+      <c r="L33">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M33">
+        <v>0.36</v>
+      </c>
+      <c r="N33" s="3">
+        <v>0.83</v>
+      </c>
+      <c r="O33" s="4">
+        <v>11</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>2.1</v>
+      </c>
+      <c r="R33">
+        <v>3.2</v>
+      </c>
+      <c r="S33">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="T33">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="U33">
+        <v>2.6</v>
+      </c>
+      <c r="V33">
+        <v>2.1</v>
+      </c>
+      <c r="W33">
+        <v>3.3</v>
+      </c>
+      <c r="X33">
+        <v>26.5</v>
+      </c>
+      <c r="Y33">
+        <v>19.8</v>
+      </c>
+      <c r="Z33">
+        <v>35.4</v>
+      </c>
+      <c r="AA33">
+        <v>29.3</v>
+      </c>
+      <c r="AB33">
+        <v>24.8</v>
+      </c>
+      <c r="AC33">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="AD33">
+        <v>46.9</v>
+      </c>
+      <c r="AE33">
+        <v>2192</v>
+      </c>
+      <c r="AF33">
+        <v>1.52E-2</v>
+      </c>
+      <c r="AG33">
+        <v>3.0870000000000002</v>
+      </c>
+      <c r="AH33">
+        <v>2191</v>
+      </c>
+      <c r="AI33">
+        <v>61.8</v>
+      </c>
+      <c r="AJ33">
+        <v>386.2</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL33" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM33" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN33">
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="AO33">
+        <v>18.8</v>
+      </c>
+      <c r="AP33">
+        <v>0.5</v>
+      </c>
+      <c r="AQ33">
+        <v>0.66</v>
+      </c>
+      <c r="AR33">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AS33">
+        <v>1.07</v>
+      </c>
+      <c r="AT33">
+        <v>0.77</v>
+      </c>
+      <c r="AU33">
+        <v>2.14</v>
+      </c>
+      <c r="AV33">
+        <v>18.8</v>
+      </c>
+      <c r="AW33">
+        <v>3.5</v>
+      </c>
+      <c r="AX33">
+        <v>0.37</v>
+      </c>
+      <c r="AY33">
+        <v>6.3</v>
+      </c>
+      <c r="AZ33">
+        <v>2191.6</v>
+      </c>
+      <c r="BA33">
+        <v>25</v>
+      </c>
+      <c r="BB33">
+        <v>1.32</v>
+      </c>
+      <c r="BC33" t="s">
+        <v>123</v>
+      </c>
+      <c r="BD33" s="8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="34" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>268</v>
+      </c>
+      <c r="B34" t="s">
+        <v>292</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>25</v>
+      </c>
+      <c r="F34">
+        <v>60</v>
+      </c>
+      <c r="G34">
+        <v>62.2</v>
+      </c>
+      <c r="H34" t="s">
+        <v>115</v>
+      </c>
+      <c r="I34" t="s">
+        <v>115</v>
+      </c>
+      <c r="J34" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="K34" t="s">
+        <v>115</v>
+      </c>
+      <c r="L34">
+        <v>0.39</v>
+      </c>
+      <c r="M34">
+        <v>0.26</v>
+      </c>
+      <c r="N34" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="O34" s="4">
+        <v>15.9</v>
+      </c>
+      <c r="P34">
+        <v>1.4</v>
+      </c>
+      <c r="Q34">
+        <v>2.9</v>
+      </c>
+      <c r="R34">
+        <v>4.8</v>
+      </c>
+      <c r="S34">
+        <v>3.5</v>
+      </c>
+      <c r="T34">
+        <v>6.9</v>
+      </c>
+      <c r="U34">
+        <v>3.6</v>
+      </c>
+      <c r="V34">
+        <v>2.9</v>
+      </c>
+      <c r="W34">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="X34">
+        <v>34.1</v>
+      </c>
+      <c r="Y34">
+        <v>25.5</v>
+      </c>
+      <c r="Z34">
+        <v>45.7</v>
+      </c>
+      <c r="AA34">
+        <v>39.4</v>
+      </c>
+      <c r="AB34">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="AC34">
+        <v>46.6</v>
+      </c>
+      <c r="AD34" s="4">
+        <v>62.2</v>
+      </c>
+      <c r="AE34">
+        <v>5373</v>
+      </c>
+      <c r="AF34">
+        <v>3.9800000000000002E-2</v>
+      </c>
+      <c r="AG34" s="6">
+        <v>2.86</v>
+      </c>
+      <c r="AH34" s="7">
+        <v>5371</v>
+      </c>
+      <c r="AI34">
+        <v>155.6</v>
+      </c>
+      <c r="AJ34">
+        <v>972.5</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL34" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM34" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN34">
+        <v>2.46E-2</v>
+      </c>
+      <c r="AO34">
+        <v>24.9</v>
+      </c>
+      <c r="AP34">
+        <v>0.5</v>
+      </c>
+      <c r="AQ34">
+        <v>0.66</v>
+      </c>
+      <c r="AR34">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AS34">
+        <v>0.76</v>
+      </c>
+      <c r="AT34">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AU34">
+        <v>1.52</v>
+      </c>
+      <c r="AV34">
+        <v>24.9</v>
+      </c>
+      <c r="AW34">
+        <v>4</v>
+      </c>
+      <c r="AX34">
+        <v>0.66</v>
+      </c>
+      <c r="AY34">
+        <v>5.3</v>
+      </c>
+      <c r="AZ34">
+        <v>5371.8</v>
+      </c>
+      <c r="BA34">
+        <v>25</v>
+      </c>
+      <c r="BB34">
+        <v>1.32</v>
+      </c>
+      <c r="BC34" t="s">
+        <v>123</v>
+      </c>
+      <c r="BD34" s="8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="35" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>269</v>
+      </c>
+      <c r="B35" t="s">
+        <v>296</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>25</v>
+      </c>
+      <c r="F35">
+        <v>34</v>
+      </c>
+      <c r="G35">
+        <v>26.5</v>
+      </c>
+      <c r="H35" t="s">
+        <v>115</v>
+      </c>
+      <c r="I35" t="s">
+        <v>115</v>
+      </c>
+      <c r="J35" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="K35">
+        <v>2.62</v>
+      </c>
+      <c r="L35">
+        <v>1.19</v>
+      </c>
+      <c r="M35">
+        <v>0.79</v>
+      </c>
+      <c r="N35" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="O35" s="4">
+        <v>4.8</v>
+      </c>
+      <c r="P35" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>115</v>
+      </c>
+      <c r="R35">
+        <v>1.3</v>
+      </c>
+      <c r="S35" t="s">
+        <v>115</v>
+      </c>
+      <c r="T35" t="s">
+        <v>115</v>
+      </c>
+      <c r="U35">
+        <v>1.3</v>
+      </c>
+      <c r="V35" t="s">
+        <v>115</v>
+      </c>
+      <c r="W35" t="s">
+        <v>115</v>
+      </c>
+      <c r="X35">
+        <v>15.8</v>
+      </c>
+      <c r="Y35">
+        <v>11.8</v>
+      </c>
+      <c r="Z35">
+        <v>21.2</v>
+      </c>
+      <c r="AA35">
+        <v>16.2</v>
+      </c>
+      <c r="AB35">
+        <v>13.7</v>
+      </c>
+      <c r="AC35">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="AD35">
+        <v>26.5</v>
+      </c>
+      <c r="AE35">
+        <v>743</v>
+      </c>
+      <c r="AF35">
+        <v>3.9300000000000002E-2</v>
+      </c>
+      <c r="AG35">
+        <v>3.0049999999999999</v>
+      </c>
+      <c r="AH35">
+        <v>744</v>
+      </c>
+      <c r="AI35">
+        <v>20.3</v>
+      </c>
+      <c r="AJ35">
+        <v>126.8</v>
+      </c>
+      <c r="AK35" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL35" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM35" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN35">
+        <v>2.7799999999999998E-2</v>
+      </c>
+      <c r="AO35">
+        <v>10.6</v>
+      </c>
+      <c r="AP35">
+        <v>0.5</v>
+      </c>
+      <c r="AQ35">
+        <v>0.64</v>
+      </c>
+      <c r="AR35">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AS35">
+        <v>2.12</v>
+      </c>
+      <c r="AT35">
+        <v>1.6</v>
+      </c>
+      <c r="AU35">
+        <v>4.24</v>
+      </c>
+      <c r="AV35">
+        <v>10.6</v>
+      </c>
+      <c r="AW35">
+        <v>2</v>
+      </c>
+      <c r="AX35" t="s">
+        <v>115</v>
+      </c>
+      <c r="AY35">
+        <v>21.2</v>
+      </c>
+      <c r="AZ35">
+        <v>743.4</v>
+      </c>
+      <c r="BA35">
+        <v>26.4</v>
+      </c>
+      <c r="BB35">
+        <v>1.32</v>
+      </c>
+      <c r="BC35" t="s">
+        <v>116</v>
+      </c>
+      <c r="BD35" s="8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="36" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>270</v>
+      </c>
+      <c r="B36" t="s">
+        <v>300</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36">
+        <v>6</v>
+      </c>
+      <c r="E36">
+        <v>15</v>
+      </c>
+      <c r="F36">
+        <v>51</v>
+      </c>
+      <c r="G36">
+        <v>53</v>
+      </c>
+      <c r="H36" t="s">
+        <v>115</v>
+      </c>
+      <c r="I36" t="s">
+        <v>115</v>
+      </c>
+      <c r="J36" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="K36" t="s">
+        <v>115</v>
+      </c>
+      <c r="L36">
+        <v>0.66</v>
+      </c>
+      <c r="M36">
+        <v>0.44</v>
+      </c>
+      <c r="N36" s="3">
+        <v>1</v>
+      </c>
+      <c r="O36" s="4">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="P36">
+        <v>0.7</v>
+      </c>
+      <c r="Q36">
+        <v>1.5</v>
+      </c>
+      <c r="R36">
+        <v>2.4</v>
+      </c>
+      <c r="S36">
+        <v>1.8</v>
+      </c>
+      <c r="T36">
+        <v>3.5</v>
+      </c>
+      <c r="U36">
+        <v>1.9</v>
+      </c>
+      <c r="V36">
+        <v>1.5</v>
+      </c>
+      <c r="W36">
+        <v>2.4</v>
+      </c>
+      <c r="X36">
+        <v>29.5</v>
+      </c>
+      <c r="Y36">
+        <v>22</v>
+      </c>
+      <c r="Z36">
+        <v>39.6</v>
+      </c>
+      <c r="AA36">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="AB36">
+        <v>28.2</v>
+      </c>
+      <c r="AC36">
+        <v>39.4</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>115</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF36" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG36" t="s">
+        <v>115</v>
+      </c>
+      <c r="AH36" t="s">
+        <v>115</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ36" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK36" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL36" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM36" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN36">
+        <v>3.1E-2</v>
+      </c>
+      <c r="AO36">
+        <v>21.2</v>
+      </c>
+      <c r="AP36">
+        <v>0.5</v>
+      </c>
+      <c r="AQ36">
+        <v>0.63</v>
+      </c>
+      <c r="AR36">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AS36">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="AT36">
+        <v>0.86</v>
+      </c>
+      <c r="AU36">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="AV36">
+        <v>21.2</v>
+      </c>
+      <c r="AW36">
+        <v>2</v>
+      </c>
+      <c r="AX36" t="s">
+        <v>115</v>
+      </c>
+      <c r="AY36">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="AZ36">
+        <v>1488.8</v>
+      </c>
+      <c r="BA36">
+        <v>25</v>
+      </c>
+      <c r="BB36">
+        <v>1.32</v>
+      </c>
+      <c r="BC36" t="s">
+        <v>116</v>
+      </c>
+      <c r="BD36" s="8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="37" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>271</v>
+      </c>
+      <c r="B37" t="s">
+        <v>302</v>
+      </c>
+      <c r="C37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>30</v>
+      </c>
+      <c r="F37">
+        <v>40</v>
+      </c>
+      <c r="G37">
+        <v>41.7</v>
+      </c>
+      <c r="H37" t="s">
+        <v>115</v>
+      </c>
+      <c r="I37" t="s">
+        <v>115</v>
+      </c>
+      <c r="J37" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="K37" t="s">
+        <v>115</v>
+      </c>
+      <c r="L37">
+        <v>0.96</v>
+      </c>
+      <c r="M37">
+        <v>0.64</v>
+      </c>
+      <c r="N37" s="3">
+        <v>1.46</v>
+      </c>
+      <c r="O37" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="P37">
+        <v>0.5</v>
+      </c>
+      <c r="Q37">
+        <v>1</v>
+      </c>
+      <c r="R37">
+        <v>1.6</v>
+      </c>
+      <c r="S37">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T37">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="U37">
+        <v>1.3</v>
+      </c>
+      <c r="V37">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="W37">
+        <v>1.7</v>
+      </c>
+      <c r="X37">
+        <v>23.8</v>
+      </c>
+      <c r="Y37">
+        <v>17.8</v>
+      </c>
+      <c r="Z37">
+        <v>31.9</v>
+      </c>
+      <c r="AA37">
+        <v>26</v>
+      </c>
+      <c r="AB37">
+        <v>21.9</v>
+      </c>
+      <c r="AC37">
+        <v>30.7</v>
+      </c>
+      <c r="AD37">
+        <v>41.7</v>
+      </c>
+      <c r="AE37">
+        <v>711</v>
+      </c>
+      <c r="AF37">
+        <v>4.41E-2</v>
+      </c>
+      <c r="AG37">
+        <v>2.6970000000000001</v>
+      </c>
+      <c r="AH37">
+        <v>711</v>
+      </c>
+      <c r="AI37">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="AJ37">
+        <v>121.2</v>
+      </c>
+      <c r="AK37" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL37" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM37" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN37">
+        <v>3.2099999999999997E-2</v>
+      </c>
+      <c r="AO37">
+        <v>16.7</v>
+      </c>
+      <c r="AP37">
+        <v>0.5</v>
+      </c>
+      <c r="AQ37">
+        <v>0.63</v>
+      </c>
+      <c r="AR37">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AS37">
+        <v>1.63</v>
+      </c>
+      <c r="AT37">
+        <v>1.25</v>
+      </c>
+      <c r="AU37">
+        <v>3.26</v>
+      </c>
+      <c r="AV37">
+        <v>16.7</v>
+      </c>
+      <c r="AW37">
+        <v>2.7</v>
+      </c>
+      <c r="AX37">
+        <v>0.3</v>
+      </c>
+      <c r="AY37">
+        <v>28.5</v>
+      </c>
+      <c r="AZ37">
+        <v>711.1</v>
+      </c>
+      <c r="BA37">
+        <v>26</v>
+      </c>
+      <c r="BB37">
+        <v>1.32</v>
+      </c>
+      <c r="BC37" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD37" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="BD21" r:id="rId1" xr:uid="{0855E8CE-BF5D-FE4C-B242-2206D93E6385}"/>
@@ -5904,6 +7730,16 @@
     <hyperlink ref="BD25" r:id="rId24" xr:uid="{09FB9F76-3AF0-CA43-85C7-BBBDA3AA1192}"/>
     <hyperlink ref="BD26" r:id="rId25" xr:uid="{01D1F225-7340-2443-B7A0-0E60B60F02C2}"/>
     <hyperlink ref="BD27" r:id="rId26" xr:uid="{95218792-52ED-4F47-8230-79B878773FBF}"/>
+    <hyperlink ref="BD28" r:id="rId27" xr:uid="{23660627-E7C9-9B44-94F8-A0C5550E81D8}"/>
+    <hyperlink ref="BD29" r:id="rId28" xr:uid="{494C7E08-B3AB-4B4A-8B88-C4023BA527BF}"/>
+    <hyperlink ref="BD30" r:id="rId29" xr:uid="{4F05D4D9-AD94-FB41-8980-4371A99C6221}"/>
+    <hyperlink ref="BD31" r:id="rId30" xr:uid="{69D2B949-ED48-8840-AAF1-C7398AAFC812}"/>
+    <hyperlink ref="BD32" r:id="rId31" xr:uid="{8A1C58B0-251A-7D47-A690-86494D3B5334}"/>
+    <hyperlink ref="BD33" r:id="rId32" xr:uid="{08E40663-8061-4741-B22C-82DA677D4C96}"/>
+    <hyperlink ref="BD34" r:id="rId33" xr:uid="{B3543BF1-462B-6D47-B934-C317B44FE158}"/>
+    <hyperlink ref="BD35" r:id="rId34" xr:uid="{E523DEF4-4A3E-CD4F-AB28-8C8FCA4FCB05}"/>
+    <hyperlink ref="BD36" r:id="rId35" xr:uid="{2EDD6381-2F42-1549-B2F4-56D7D2D59E3F}"/>
+    <hyperlink ref="BD37" r:id="rId36" xr:uid="{9A47CF8B-C962-FE40-8CFC-0BF0DE9D6FBC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5911,15 +7747,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8401CC-45AA-794F-825D-4F3F9F3C5EA7}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D31" sqref="D31:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="60.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -6234,14 +8070,14 @@
       <c r="C10" t="s">
         <v>115</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>1.0840000000000001</v>
+      <c r="D10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" t="s">
+        <v>115</v>
       </c>
       <c r="F10" t="s">
-        <v>215</v>
+        <v>115</v>
       </c>
       <c r="G10" t="s">
         <v>115</v>
@@ -6557,20 +8393,20 @@
       <c r="C20" t="s">
         <v>115</v>
       </c>
-      <c r="D20">
-        <v>-1.3260000000000001</v>
-      </c>
-      <c r="E20">
-        <v>0.88</v>
+      <c r="D20" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" t="s">
+        <v>115</v>
       </c>
       <c r="F20" t="s">
-        <v>215</v>
+        <v>115</v>
       </c>
       <c r="G20" t="s">
-        <v>246</v>
-      </c>
-      <c r="H20">
-        <v>0.99586699999999995</v>
+        <v>115</v>
+      </c>
+      <c r="H20" t="s">
+        <v>115</v>
       </c>
       <c r="I20" t="s">
         <v>115</v>
@@ -6579,7 +8415,7 @@
         <v>226</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -6602,7 +8438,7 @@
         <v>204</v>
       </c>
       <c r="G21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H21">
         <v>0.86</v>
@@ -6611,7 +8447,7 @@
         <v>115</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -6624,20 +8460,20 @@
       <c r="C22" t="s">
         <v>115</v>
       </c>
-      <c r="D22">
-        <v>-0.78100000000000003</v>
-      </c>
-      <c r="E22">
-        <v>0.85</v>
+      <c r="D22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" t="s">
+        <v>115</v>
       </c>
       <c r="F22" t="s">
-        <v>215</v>
+        <v>115</v>
       </c>
       <c r="G22" t="s">
-        <v>250</v>
-      </c>
-      <c r="H22">
-        <v>0.99932600000000005</v>
+        <v>115</v>
+      </c>
+      <c r="H22" t="s">
+        <v>115</v>
       </c>
       <c r="I22" t="s">
         <v>115</v>
@@ -6646,7 +8482,7 @@
         <v>226</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -6669,7 +8505,7 @@
         <v>215</v>
       </c>
       <c r="G23" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H23">
         <v>0.89</v>
@@ -6678,7 +8514,7 @@
         <v>29</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -6701,7 +8537,7 @@
         <v>204</v>
       </c>
       <c r="G24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H24">
         <v>0.99399999999999999</v>
@@ -6710,7 +8546,7 @@
         <v>247</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -6733,7 +8569,7 @@
         <v>215</v>
       </c>
       <c r="G25" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H25">
         <v>0.99</v>
@@ -6742,7 +8578,7 @@
         <v>4570</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -6765,7 +8601,7 @@
         <v>215</v>
       </c>
       <c r="G26" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H26">
         <v>0.98799999999999999</v>
@@ -6774,7 +8610,7 @@
         <v>67</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -6797,7 +8633,7 @@
         <v>215</v>
       </c>
       <c r="G27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H27">
         <v>0.90900000000000003</v>
@@ -6806,7 +8642,7 @@
         <v>736</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -6829,7 +8665,7 @@
         <v>215</v>
       </c>
       <c r="G28" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H28">
         <v>0.997</v>
@@ -6838,7 +8674,327 @@
         <v>5260</v>
       </c>
       <c r="K28" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>262</v>
+      </c>
+      <c r="B29" t="s">
+        <v>272</v>
+      </c>
+      <c r="C29">
+        <v>0.98</v>
+      </c>
+      <c r="D29">
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="E29">
+        <v>3.278</v>
+      </c>
+      <c r="F29" t="s">
+        <v>215</v>
+      </c>
+      <c r="G29" t="s">
+        <v>274</v>
+      </c>
+      <c r="H29">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="I29">
+        <v>140</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>263</v>
+      </c>
+      <c r="B30" t="s">
+        <v>276</v>
+      </c>
+      <c r="C30" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" t="s">
+        <v>115</v>
+      </c>
+      <c r="F30" t="s">
+        <v>115</v>
+      </c>
+      <c r="G30" t="s">
+        <v>115</v>
+      </c>
+      <c r="H30" t="s">
+        <v>115</v>
+      </c>
+      <c r="I30" t="s">
+        <v>115</v>
+      </c>
+      <c r="J30" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>264</v>
+      </c>
+      <c r="B31" t="s">
+        <v>278</v>
+      </c>
+      <c r="C31">
+        <v>0.99</v>
+      </c>
+      <c r="D31">
+        <v>3.1199999999999999E-2</v>
+      </c>
+      <c r="E31">
+        <v>2.9529999999999998</v>
+      </c>
+      <c r="F31" t="s">
+        <v>215</v>
+      </c>
+      <c r="G31" t="s">
+        <v>282</v>
+      </c>
+      <c r="H31">
+        <v>0.99</v>
+      </c>
+      <c r="I31">
+        <v>74</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>265</v>
+      </c>
+      <c r="B32" t="s">
+        <v>280</v>
+      </c>
+      <c r="C32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" t="s">
+        <v>115</v>
+      </c>
+      <c r="G32" t="s">
+        <v>115</v>
+      </c>
+      <c r="H32" t="s">
+        <v>115</v>
+      </c>
+      <c r="I32" t="s">
+        <v>115</v>
+      </c>
+      <c r="J32" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>266</v>
+      </c>
+      <c r="B33" t="s">
+        <v>284</v>
+      </c>
+      <c r="C33">
+        <v>0.98</v>
+      </c>
+      <c r="D33">
+        <v>1.6E-2</v>
+      </c>
+      <c r="E33">
+        <v>3.077</v>
+      </c>
+      <c r="F33" t="s">
+        <v>290</v>
+      </c>
+      <c r="G33" t="s">
+        <v>115</v>
+      </c>
+      <c r="H33">
+        <v>0.98</v>
+      </c>
+      <c r="I33">
+        <v>76</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>267</v>
+      </c>
+      <c r="B34" t="s">
+        <v>286</v>
+      </c>
+      <c r="C34">
+        <v>0.98</v>
+      </c>
+      <c r="D34">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="E34">
+        <v>2.92</v>
+      </c>
+      <c r="F34" t="s">
+        <v>215</v>
+      </c>
+      <c r="G34" t="s">
+        <v>288</v>
+      </c>
+      <c r="H34">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="I34">
+        <v>323</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>268</v>
+      </c>
+      <c r="B35" t="s">
+        <v>292</v>
+      </c>
+      <c r="C35">
+        <v>0.95</v>
+      </c>
+      <c r="D35">
+        <v>3.9800000000000002E-2</v>
+      </c>
+      <c r="E35">
+        <v>2.86</v>
+      </c>
+      <c r="F35" t="s">
+        <v>215</v>
+      </c>
+      <c r="G35" t="s">
+        <v>294</v>
+      </c>
+      <c r="H35">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="I35">
+        <v>16</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>269</v>
+      </c>
+      <c r="B36" t="s">
+        <v>296</v>
+      </c>
+      <c r="C36">
+        <v>0.97</v>
+      </c>
+      <c r="D36">
+        <v>1.41E-2</v>
+      </c>
+      <c r="E36">
+        <v>3.14</v>
+      </c>
+      <c r="F36" t="s">
+        <v>215</v>
+      </c>
+      <c r="G36" t="s">
+        <v>298</v>
+      </c>
+      <c r="H36">
+        <v>0.97</v>
+      </c>
+      <c r="I36">
+        <v>209</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>270</v>
+      </c>
+      <c r="B37" t="s">
+        <v>300</v>
+      </c>
+      <c r="C37" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" t="s">
+        <v>115</v>
+      </c>
+      <c r="F37" t="s">
+        <v>115</v>
+      </c>
+      <c r="G37" t="s">
+        <v>115</v>
+      </c>
+      <c r="H37" t="s">
+        <v>115</v>
+      </c>
+      <c r="I37" t="s">
+        <v>115</v>
+      </c>
+      <c r="J37" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>271</v>
+      </c>
+      <c r="B38" t="s">
+        <v>302</v>
+      </c>
+      <c r="C38">
+        <v>0.99</v>
+      </c>
+      <c r="D38">
+        <v>4.41E-2</v>
+      </c>
+      <c r="E38">
+        <v>2.597</v>
+      </c>
+      <c r="F38" t="s">
+        <v>215</v>
+      </c>
+      <c r="G38" t="s">
+        <v>304</v>
+      </c>
+      <c r="H38">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="I38">
+        <v>64</v>
+      </c>
+      <c r="K38" s="8" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -6870,6 +9026,13 @@
     <hyperlink ref="K26" r:id="rId25" xr:uid="{339C461A-9B2A-3042-81B0-713633982DD9}"/>
     <hyperlink ref="K27" r:id="rId26" xr:uid="{80F7FB94-CB99-7F4F-89EC-A0676B20F509}"/>
     <hyperlink ref="K28" r:id="rId27" xr:uid="{0018D18B-4CF2-F643-9FF2-61C2355BF2C6}"/>
+    <hyperlink ref="K29" r:id="rId28" xr:uid="{8E9151CE-32D9-C24B-AF38-7000C6F984F9}"/>
+    <hyperlink ref="K31" r:id="rId29" xr:uid="{F38C22EA-7CFC-8C40-ADE9-F891EB158215}"/>
+    <hyperlink ref="K34" r:id="rId30" xr:uid="{CC867BD3-8EF6-9D48-B207-17DA1A4F9334}"/>
+    <hyperlink ref="K33" r:id="rId31" xr:uid="{006C10E8-3F87-5543-A5CA-F6E79A0ED450}"/>
+    <hyperlink ref="K35" r:id="rId32" xr:uid="{02A4312A-02B7-1A42-B567-00DB9639614C}"/>
+    <hyperlink ref="K36" r:id="rId33" xr:uid="{1D7C0C62-2B5C-F343-9D46-0DC5D3214AD7}"/>
+    <hyperlink ref="K38" r:id="rId34" xr:uid="{E9C67390-AA73-634F-AD33-4E827C3BE18A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>